<commit_message>
21.06.2018_Second Commit after importing environment and the scenario logic
</commit_message>
<xml_diff>
--- a/Resources/Data/DataSheet.xlsx
+++ b/Resources/Data/DataSheet.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Robot_Vijoy\OMS_Regression\Resources\Data\SKU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Robot_Vijoy\OMS_Regression\Resources\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7050" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7050" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Environment" sheetId="9" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2350" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2467" uniqueCount="396">
   <si>
     <t>S.No</t>
   </si>
@@ -1108,12 +1108,162 @@
   <si>
     <t>89001</t>
   </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Value1</t>
+  </si>
+  <si>
+    <t>Value2</t>
+  </si>
+  <si>
+    <t>Value3</t>
+  </si>
+  <si>
+    <t>Value4</t>
+  </si>
+  <si>
+    <t>Value5</t>
+  </si>
+  <si>
+    <t>Value8</t>
+  </si>
+  <si>
+    <t>Value9</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>SIT</t>
+  </si>
+  <si>
+    <t>UAT</t>
+  </si>
+  <si>
+    <t>OMS_9.5_Prod</t>
+  </si>
+  <si>
+    <t>FVT</t>
+  </si>
+  <si>
+    <t>SFS_CSIT</t>
+  </si>
+  <si>
+    <t>SFS_CSIT_New</t>
+  </si>
+  <si>
+    <t>SFS_DSIT</t>
+  </si>
+  <si>
+    <t>SFS_DSIT_New</t>
+  </si>
+  <si>
+    <t>Execution Flag</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Y</t>
+  </si>
+  <si>
+    <t>Server Name</t>
+  </si>
+  <si>
+    <t>172.27.97.146</t>
+  </si>
+  <si>
+    <t>cmsomsappu01</t>
+  </si>
+  <si>
+    <t>ddcomsasp01vmXXX</t>
+  </si>
+  <si>
+    <t>172.27.97.135</t>
+  </si>
+  <si>
+    <t>172.26.64.42</t>
+  </si>
+  <si>
+    <t>cmsomsappt01</t>
+  </si>
+  <si>
+    <t>ddcomsast01vm</t>
+  </si>
+  <si>
+    <t>172.27.32.190</t>
+  </si>
+  <si>
+    <t>Port Number</t>
+  </si>
+  <si>
+    <t>9080</t>
+  </si>
+  <si>
+    <t>Protocol</t>
+  </si>
+  <si>
+    <t>http</t>
+  </si>
+  <si>
+    <t>Path</t>
+  </si>
+  <si>
+    <t>/smcfs/interop/InteropHttpServlet</t>
+  </si>
+  <si>
+    <t>Scenario Description</t>
+  </si>
+  <si>
+    <t>Order Type</t>
+  </si>
+  <si>
+    <t>Item Type</t>
+  </si>
+  <si>
+    <t>Shipping Address</t>
+  </si>
+  <si>
+    <t>Shipment type</t>
+  </si>
+  <si>
+    <t>Number of Orders</t>
+  </si>
+  <si>
+    <t>Order Flow</t>
+  </si>
+  <si>
+    <t>To Be Executed</t>
+  </si>
+  <si>
+    <t>#Line Items</t>
+  </si>
+  <si>
+    <t>Service Flag</t>
+  </si>
+  <si>
+    <t>Verify whether Petco order with Single_ Line item and Visa is shipped to DC associated with Northeast MA region</t>
+  </si>
+  <si>
+    <t>Petco</t>
+  </si>
+  <si>
+    <t>Single_ Line</t>
+  </si>
+  <si>
+    <t>Full Shipment</t>
+  </si>
+  <si>
+    <t>Order Life Cycle</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1157,6 +1307,19 @@
       <color rgb="FF000000"/>
       <name val="Segoe UI"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="14">
@@ -1239,7 +1402,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -1273,11 +1436,116 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1383,11 +1651,291 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="13" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="9" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="8" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <colors>
     <mruColors>
@@ -1696,26 +2244,500 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="9.42578125" customWidth="1"/>
+    <col min="2" max="2" width="20.7109375" style="49" customWidth="1"/>
+    <col min="3" max="3" width="48.7109375" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="48.5703125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="56.42578125" hidden="1" customWidth="1"/>
+    <col min="6" max="9" width="50" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="26.28515625" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="40" customWidth="1"/>
+    <col min="13" max="13" width="32.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="45" t="s">
+        <v>346</v>
+      </c>
+      <c r="C1" s="45" t="s">
+        <v>347</v>
+      </c>
+      <c r="D1" s="45" t="s">
+        <v>348</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>349</v>
+      </c>
+      <c r="F1" s="45" t="s">
+        <v>350</v>
+      </c>
+      <c r="G1" s="45" t="s">
+        <v>351</v>
+      </c>
+      <c r="H1" s="45" t="s">
+        <v>351</v>
+      </c>
+      <c r="I1" s="45" t="s">
+        <v>351</v>
+      </c>
+      <c r="J1" s="45" t="s">
+        <v>351</v>
+      </c>
+      <c r="K1" s="45" t="s">
+        <v>352</v>
+      </c>
+      <c r="L1" s="45" t="s">
+        <v>353</v>
+      </c>
+      <c r="M1" s="45" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="46">
+        <v>1</v>
+      </c>
+      <c r="B2" s="47" t="s">
+        <v>354</v>
+      </c>
+      <c r="C2" s="48" t="s">
+        <v>355</v>
+      </c>
+      <c r="D2" s="48" t="s">
+        <v>356</v>
+      </c>
+      <c r="E2" s="48" t="s">
+        <v>357</v>
+      </c>
+      <c r="F2" s="48" t="s">
+        <v>358</v>
+      </c>
+      <c r="G2" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="H2" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="I2" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="J2" s="48" t="s">
+        <v>359</v>
+      </c>
+      <c r="K2" s="48" t="s">
+        <v>360</v>
+      </c>
+      <c r="L2" s="48" t="s">
+        <v>361</v>
+      </c>
+      <c r="M2" s="48" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="46">
+        <v>2</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>363</v>
+      </c>
+      <c r="C3" s="46" t="s">
+        <v>364</v>
+      </c>
+      <c r="D3" s="46" t="s">
+        <v>364</v>
+      </c>
+      <c r="E3" s="46" t="s">
+        <v>364</v>
+      </c>
+      <c r="F3" s="46" t="s">
+        <v>364</v>
+      </c>
+      <c r="G3" s="46" t="s">
+        <v>364</v>
+      </c>
+      <c r="H3" s="46" t="s">
+        <v>364</v>
+      </c>
+      <c r="I3" s="46" t="s">
+        <v>364</v>
+      </c>
+      <c r="J3" s="46" t="s">
+        <v>364</v>
+      </c>
+      <c r="K3" s="46" t="s">
+        <v>365</v>
+      </c>
+      <c r="L3" s="46" t="s">
+        <v>364</v>
+      </c>
+      <c r="M3" s="46" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="46">
+        <v>3</v>
+      </c>
+      <c r="B4" s="47" t="s">
+        <v>366</v>
+      </c>
+      <c r="C4" s="46" t="s">
+        <v>367</v>
+      </c>
+      <c r="D4" s="46" t="s">
+        <v>368</v>
+      </c>
+      <c r="E4" s="46" t="s">
+        <v>369</v>
+      </c>
+      <c r="F4" s="46" t="s">
+        <v>370</v>
+      </c>
+      <c r="G4" s="46" t="s">
+        <v>371</v>
+      </c>
+      <c r="H4" s="46" t="s">
+        <v>371</v>
+      </c>
+      <c r="I4" s="46" t="s">
+        <v>371</v>
+      </c>
+      <c r="J4" s="46" t="s">
+        <v>371</v>
+      </c>
+      <c r="K4" s="46" t="s">
+        <v>372</v>
+      </c>
+      <c r="L4" s="46" t="s">
+        <v>373</v>
+      </c>
+      <c r="M4" s="46" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="46">
+        <v>4</v>
+      </c>
+      <c r="B5" s="47" t="s">
+        <v>375</v>
+      </c>
+      <c r="C5" s="46">
+        <v>9080</v>
+      </c>
+      <c r="D5" s="46">
+        <v>9080</v>
+      </c>
+      <c r="E5" s="46" t="s">
+        <v>376</v>
+      </c>
+      <c r="F5" s="46" t="s">
+        <v>376</v>
+      </c>
+      <c r="G5" s="46" t="s">
+        <v>376</v>
+      </c>
+      <c r="H5" s="46" t="s">
+        <v>376</v>
+      </c>
+      <c r="I5" s="46" t="s">
+        <v>376</v>
+      </c>
+      <c r="J5" s="46" t="s">
+        <v>376</v>
+      </c>
+      <c r="K5" s="46" t="s">
+        <v>376</v>
+      </c>
+      <c r="L5" s="46" t="s">
+        <v>376</v>
+      </c>
+      <c r="M5" s="46" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="46">
+        <v>5</v>
+      </c>
+      <c r="B6" s="47" t="s">
+        <v>377</v>
+      </c>
+      <c r="C6" s="46" t="s">
+        <v>378</v>
+      </c>
+      <c r="D6" s="46" t="s">
+        <v>378</v>
+      </c>
+      <c r="E6" s="46" t="s">
+        <v>378</v>
+      </c>
+      <c r="F6" s="46" t="s">
+        <v>378</v>
+      </c>
+      <c r="G6" s="46" t="s">
+        <v>378</v>
+      </c>
+      <c r="H6" s="46" t="s">
+        <v>378</v>
+      </c>
+      <c r="I6" s="46" t="s">
+        <v>378</v>
+      </c>
+      <c r="J6" s="46" t="s">
+        <v>378</v>
+      </c>
+      <c r="K6" s="46" t="s">
+        <v>378</v>
+      </c>
+      <c r="L6" s="46" t="s">
+        <v>378</v>
+      </c>
+      <c r="M6" s="46" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="46">
+        <v>6</v>
+      </c>
+      <c r="B7" s="47" t="s">
+        <v>379</v>
+      </c>
+      <c r="C7" s="46" t="s">
+        <v>380</v>
+      </c>
+      <c r="D7" s="46" t="s">
+        <v>380</v>
+      </c>
+      <c r="E7" s="46" t="s">
+        <v>380</v>
+      </c>
+      <c r="F7" s="46" t="s">
+        <v>380</v>
+      </c>
+      <c r="G7" s="46" t="s">
+        <v>380</v>
+      </c>
+      <c r="H7" s="46" t="s">
+        <v>380</v>
+      </c>
+      <c r="I7" s="46" t="s">
+        <v>380</v>
+      </c>
+      <c r="J7" s="46" t="s">
+        <v>380</v>
+      </c>
+      <c r="K7" s="46" t="s">
+        <v>380</v>
+      </c>
+      <c r="L7" s="46" t="s">
+        <v>380</v>
+      </c>
+      <c r="M7" s="46" t="s">
+        <v>380</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C3:F3">
+    <cfRule type="containsText" dxfId="22" priority="7" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",C3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="8" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",C3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G3:K3">
+    <cfRule type="containsText" dxfId="20" priority="5" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",G3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="6" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",G3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L3">
+    <cfRule type="containsText" dxfId="18" priority="3" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",L3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="4" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",L3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M3">
+    <cfRule type="containsText" dxfId="16" priority="1" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",M3)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="15" priority="2" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",M3)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="23.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="92.5703125" customWidth="1"/>
+    <col min="3" max="3" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="51" t="s">
+        <v>381</v>
+      </c>
+      <c r="C1" s="52" t="s">
+        <v>382</v>
+      </c>
+      <c r="D1" s="52" t="s">
+        <v>383</v>
+      </c>
+      <c r="E1" s="52" t="s">
+        <v>384</v>
+      </c>
+      <c r="F1" s="52" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="52" t="s">
+        <v>385</v>
+      </c>
+      <c r="H1" s="52" t="s">
+        <v>386</v>
+      </c>
+      <c r="I1" s="52" t="s">
+        <v>387</v>
+      </c>
+      <c r="J1" s="52" t="s">
+        <v>388</v>
+      </c>
+      <c r="K1" s="52" t="s">
+        <v>389</v>
+      </c>
+      <c r="L1" s="53" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="54">
+        <v>1</v>
+      </c>
+      <c r="B2" s="55" t="s">
+        <v>391</v>
+      </c>
+      <c r="C2" s="56" t="s">
+        <v>392</v>
+      </c>
+      <c r="D2" s="56" t="s">
+        <v>393</v>
+      </c>
+      <c r="E2" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" s="56" t="s">
+        <v>394</v>
+      </c>
+      <c r="H2" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="I2" s="59" t="s">
+        <v>395</v>
+      </c>
+      <c r="J2" s="60" t="s">
+        <v>365</v>
+      </c>
+      <c r="K2" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="L2" s="61" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="54">
+        <v>2</v>
+      </c>
+      <c r="B3" s="55" t="s">
+        <v>391</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>392</v>
+      </c>
+      <c r="D3" s="56" t="s">
+        <v>393</v>
+      </c>
+      <c r="E3" s="57" t="s">
+        <v>62</v>
+      </c>
+      <c r="F3" s="56" t="s">
+        <v>5</v>
+      </c>
+      <c r="G3" s="56" t="s">
+        <v>394</v>
+      </c>
+      <c r="H3" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="I3" s="59" t="s">
+        <v>395</v>
+      </c>
+      <c r="J3" s="60" t="s">
+        <v>365</v>
+      </c>
+      <c r="K3" s="58" t="s">
+        <v>46</v>
+      </c>
+      <c r="L3" s="61" t="s">
+        <v>365</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="J1">
+    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",J1)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",J1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J1:J1048576">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",J1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I2:I3">
+      <formula1>"Order Only, Order Life Cycle"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J1:J3">
+      <formula1>"Y,N"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9998,7 +11020,7 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>

</xml_diff>